<commit_message>
migrating everything to new vps
</commit_message>
<xml_diff>
--- a/extract_load_scripts/get_tickers/input/ticker_list.xlsx
+++ b/extract_load_scripts/get_tickers/input/ticker_list.xlsx
@@ -49,7 +49,7 @@
     <t>MSCI EU SC</t>
   </si>
   <si>
-    <t>RS2K.F</t>
+    <t>RS2K.DE</t>
   </si>
   <si>
     <t>Amundi Russel 2000</t>
@@ -64,7 +64,7 @@
     <t>SP500</t>
   </si>
   <si>
-    <t>C40.PA</t>
+    <t>CACC.PA</t>
   </si>
   <si>
     <t>CAC40</t>
@@ -411,7 +411,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">

</xml_diff>